<commit_message>
Definicion Task y TaskDefinition
</commit_message>
<xml_diff>
--- a/doc/arquitectura.xlsx
+++ b/doc/arquitectura.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arquitectura" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="142">
   <si>
     <t>Componente</t>
   </si>
@@ -268,36 +268,6 @@
   </si>
   <si>
     <t>Suspended</t>
-  </si>
-  <si>
-    <t>= 1</t>
-  </si>
-  <si>
-    <t>= 2</t>
-  </si>
-  <si>
-    <t>= 3</t>
-  </si>
-  <si>
-    <t>= 4</t>
-  </si>
-  <si>
-    <t>= 5</t>
-  </si>
-  <si>
-    <t>= 6</t>
-  </si>
-  <si>
-    <t>= 7</t>
-  </si>
-  <si>
-    <t>= 8</t>
-  </si>
-  <si>
-    <t>= 9</t>
-  </si>
-  <si>
-    <t>= 10</t>
   </si>
   <si>
     <t>Extend</t>
@@ -605,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -631,6 +601,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1419,15 +1392,15 @@
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="21.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="64" customWidth="1"/>
-    <col min="12" max="12" width="19.21875" customWidth="1"/>
-    <col min="13" max="13" width="15.21875" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1441,7 +1414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
         <v>8</v>
       </c>
@@ -1455,7 +1428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J5" t="s">
         <v>7</v>
       </c>
@@ -1469,7 +1442,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
         <v>11</v>
       </c>
@@ -1480,7 +1453,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
         <v>12</v>
       </c>
@@ -1494,7 +1467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J8" t="s">
         <v>15</v>
       </c>
@@ -1508,12 +1481,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
         <v>21</v>
       </c>
@@ -1529,19 +1502,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="38" style="5" customWidth="1"/>
-    <col min="3" max="6" width="27.6640625" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="5"/>
+    <col min="3" max="6" width="27.7109375" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="11.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1532,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
@@ -1569,7 +1542,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>22</v>
       </c>
@@ -1586,7 +1559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>23</v>
       </c>
@@ -1594,7 +1567,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1602,7 +1575,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1610,7 +1583,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
@@ -1618,7 +1591,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1626,7 +1599,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1634,7 +1607,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>29</v>
       </c>
@@ -1642,7 +1615,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>41</v>
       </c>
@@ -1656,9 +1629,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1666,92 +1639,92 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>46</v>
@@ -1760,28 +1733,28 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>47</v>
@@ -1790,65 +1763,65 @@
         <v>65</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B32" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>25</v>
       </c>
@@ -1863,19 +1836,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="28.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>45</v>
       </c>
@@ -1886,10 +1859,10 @@
         <v>69</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>44</v>
       </c>
@@ -1897,143 +1870,203 @@
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="str">
+        <f>CONCATENATE("private ",C3," ",B3,";")</f>
+        <v>private long taskId;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D17" si="0">CONCATENATE("private ",C4," ",B4,";")</f>
+        <v>private long processInstanceId;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>private String name;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>private String subject;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>50</v>
       </c>
       <c r="C7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>private String description;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>51</v>
       </c>
       <c r="C8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>private Status status;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>52</v>
       </c>
       <c r="C9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>private int priority;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>53</v>
       </c>
       <c r="C10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>private boolean skipable;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>54</v>
       </c>
       <c r="C11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>private User actualOwner;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>56</v>
       </c>
       <c r="C12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>private User createBy;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>57</v>
       </c>
       <c r="C13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>private Date createdOn;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>private Date activationTime;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>60</v>
       </c>
       <c r="C15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>private Date expirationTime;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>61</v>
       </c>
       <c r="C16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>private String processId;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>63</v>
       </c>
       <c r="C17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>private int processSessionId;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>55</v>
       </c>
@@ -2042,9 +2075,9 @@
         <v>Organizational Entity</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -2053,104 +2086,144 @@
         <v>Organizational Entity</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="11">
+        <v>1</v>
+      </c>
+      <c r="D26" t="str">
+        <f>CONCATENATE(B26,"(",C26,"),")</f>
+        <v>Created(1),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="11">
+        <v>2</v>
+      </c>
+      <c r="D27" t="str">
+        <f>CONCATENATE(B27,"(",C27,"),")</f>
+        <v>Ready(2),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="11">
+        <v>3</v>
+      </c>
+      <c r="D28" t="str">
+        <f>CONCATENATE(B28,"(",C28,"),")</f>
+        <v>Reserved(3),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="11">
+        <v>4</v>
+      </c>
+      <c r="D29" t="str">
+        <f>CONCATENATE(B29,"(",C29,"),")</f>
+        <v>InProgress(4),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="11">
+        <v>5</v>
+      </c>
+      <c r="D30" t="str">
+        <f>CONCATENATE(B30,"(",C30,"),")</f>
+        <v>Suspended(5),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+      <c r="C31" s="11">
+        <v>6</v>
+      </c>
+      <c r="D31" t="str">
+        <f>CONCATENATE(B31,"(",C31,"),")</f>
+        <v>Completed(6),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="11">
+        <v>7</v>
+      </c>
+      <c r="D32" t="str">
+        <f>CONCATENATE(B32,"(",C32,"),")</f>
+        <v>Failed(7),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
+      <c r="C33" s="11">
+        <v>8</v>
+      </c>
+      <c r="D33" t="str">
+        <f>CONCATENATE(B33,"(",C33,"),")</f>
+        <v>Error(8),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+      <c r="C34" s="11">
+        <v>9</v>
+      </c>
+      <c r="D34" t="str">
+        <f>CONCATENATE(B34,"(",C34,"),")</f>
+        <v>Exited(9),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="C35" s="11">
+        <v>10</v>
+      </c>
+      <c r="D35" t="str">
+        <f>CONCATENATE(B35,"(",C35,"),")</f>
+        <v>Obsolete(10),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>50</v>
       </c>
@@ -2158,15 +2231,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>48</v>
       </c>
@@ -2174,15 +2247,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>52</v>
       </c>
@@ -2190,69 +2263,69 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C46" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C48" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>59</v>
       </c>
@@ -2260,7 +2333,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>54</v>
       </c>
@@ -2268,23 +2341,23 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C52" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C53" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>56</v>
       </c>
@@ -2292,7 +2365,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>57</v>
       </c>
@@ -2300,95 +2373,95 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C56" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C57" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C58" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C60" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C61" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C62" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C63" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C65" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C66" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>61</v>
       </c>
@@ -2396,7 +2469,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>47</v>
       </c>
@@ -2404,7 +2477,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>63</v>
       </c>
@@ -2412,7 +2485,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>51</v>
       </c>
@@ -2420,15 +2493,15 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C71" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>53</v>
       </c>
@@ -2437,6 +2510,10 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="B26:D35">
+    <sortCondition ref="C26:C35"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>